<commit_message>
update drug list to 2025 Orange Book and Purple Book, and add SMILES strings
</commit_message>
<xml_diff>
--- a/drug-list/data/02_intermediate/pmda/pmda-with-curies.xlsx
+++ b/drug-list/data/02_intermediate/pmda/pmda-with-curies.xlsx
@@ -2196,12 +2196,12 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -2801,12 +2801,12 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>UNII:3H8GSZ4SQL</t>
+          <t>UNII:GDW7M2P1IS</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Avatrombopag</t>
+          <t>AVATROMBOPAG MALEATE</t>
         </is>
       </c>
     </row>
@@ -3131,12 +3131,12 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>CHEBI:9180</t>
+          <t>CHEBI:28741</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Sodium salicylate</t>
+          <t>Sodium fluoride</t>
         </is>
       </c>
     </row>
@@ -4836,12 +4836,12 @@
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>UNII:54K37P50KH</t>
+          <t>UNII:5SML1T733B</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>Valbenazine</t>
+          <t>VALBENAZINE TOSYLATE</t>
         </is>
       </c>
     </row>
@@ -6761,12 +6761,12 @@
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr">
         <is>
-          <t>UNII:XZA0KB1BDQ</t>
+          <t>UNII:88SH1NBL2B</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>Berotralstat</t>
+          <t>Berotralstat Hydrochloride</t>
         </is>
       </c>
     </row>
@@ -6871,12 +6871,12 @@
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr">
         <is>
-          <t>CHEBI:4508</t>
+          <t>CHEBI:47381</t>
         </is>
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>diclofenac potassium</t>
+          <t>Diclofenac</t>
         </is>
       </c>
     </row>
@@ -7476,12 +7476,12 @@
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr">
         <is>
-          <t>CHEBI:6446</t>
+          <t>CHEBI:18332</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>Levothroid</t>
+          <t>Levothyroxine</t>
         </is>
       </c>
     </row>
@@ -8576,12 +8576,12 @@
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr">
         <is>
-          <t>UNII:P188ANX8CK</t>
+          <t>UNII:5384HK7574</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>Trastuzumab</t>
+          <t>Trastuzumab deruxtecan</t>
         </is>
       </c>
     </row>
@@ -8966,7 +8966,7 @@
       </c>
       <c r="M155" t="inlineStr">
         <is>
-          <t>CID 86278165</t>
+          <t>Ferric carboxymaltose</t>
         </is>
       </c>
     </row>
@@ -11821,12 +11821,12 @@
       <c r="K207" t="inlineStr"/>
       <c r="L207" t="inlineStr">
         <is>
-          <t>UNII:03KSI6WLXH</t>
+          <t>UNII:V1N8F1RVVO</t>
         </is>
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>Naldemedine</t>
+          <t>NALDEMEDINE TOSYLATE</t>
         </is>
       </c>
     </row>
@@ -11876,12 +11876,12 @@
       <c r="K208" t="inlineStr"/>
       <c r="L208" t="inlineStr">
         <is>
-          <t>CHEBI:31414</t>
+          <t>CHEBI:205919</t>
         </is>
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>Clobetasol propionate</t>
+          <t>Clobetasol</t>
         </is>
       </c>
     </row>
@@ -12041,12 +12041,12 @@
       <c r="K211" t="inlineStr"/>
       <c r="L211" t="inlineStr">
         <is>
-          <t>UNII:4O2AB118LA</t>
+          <t>CHEBI:132975</t>
         </is>
       </c>
       <c r="M211" t="inlineStr">
         <is>
-          <t>GRAZOPREVIR</t>
+          <t>Grazoprevir</t>
         </is>
       </c>
     </row>
@@ -14406,12 +14406,12 @@
       <c r="K254" t="inlineStr"/>
       <c r="L254" t="inlineStr">
         <is>
-          <t>CHEBI:26710</t>
+          <t>CHEBI:43830</t>
         </is>
       </c>
       <c r="M254" t="inlineStr">
         <is>
-          <t>Sodium chloride</t>
+          <t>Methylthioninium</t>
         </is>
       </c>
     </row>
@@ -14741,7 +14741,7 @@
       </c>
       <c r="M260" t="inlineStr">
         <is>
-          <t>Nalfurafine hydrochloride</t>
+          <t>Nalfurafine Hydrochloride</t>
         </is>
       </c>
     </row>
@@ -15121,12 +15121,12 @@
       <c r="K267" t="inlineStr"/>
       <c r="L267" t="inlineStr">
         <is>
-          <t>CHEBI:34650</t>
+          <t>CHEBI:37943</t>
         </is>
       </c>
       <c r="M267" t="inlineStr">
         <is>
-          <t>COLISTIMETHATE</t>
+          <t>Colistin</t>
         </is>
       </c>
     </row>
@@ -15231,12 +15231,12 @@
       <c r="K269" t="inlineStr"/>
       <c r="L269" t="inlineStr">
         <is>
-          <t>CHEBI:73272</t>
+          <t>CHEBI:73274</t>
         </is>
       </c>
       <c r="M269" t="inlineStr">
         <is>
-          <t>CANAGLIFLOZIN</t>
+          <t>Canagliflozin</t>
         </is>
       </c>
     </row>
@@ -15451,12 +15451,12 @@
       <c r="K273" t="inlineStr"/>
       <c r="L273" t="inlineStr">
         <is>
-          <t>CHEBI:68639</t>
+          <t>CHEBI:68642</t>
         </is>
       </c>
       <c r="M273" t="inlineStr">
         <is>
-          <t>abiraterone acetate</t>
+          <t>Abiraterone</t>
         </is>
       </c>
     </row>
@@ -15561,12 +15561,12 @@
       <c r="K275" t="inlineStr"/>
       <c r="L275" t="inlineStr">
         <is>
-          <t>CHEBI:66917</t>
+          <t>CHEBI:66919</t>
         </is>
       </c>
       <c r="M275" t="inlineStr">
         <is>
-          <t>ruxolitinib phosphate</t>
+          <t>Ruxolitinib</t>
         </is>
       </c>
     </row>
@@ -15671,12 +15671,12 @@
       <c r="K277" t="inlineStr"/>
       <c r="L277" t="inlineStr">
         <is>
-          <t>CHEBI:55345</t>
+          <t>CHEBI:142290</t>
         </is>
       </c>
       <c r="M277" t="inlineStr">
         <is>
-          <t>anagrelide hydrochloride</t>
+          <t>Anagrelide</t>
         </is>
       </c>
     </row>
@@ -16056,12 +16056,12 @@
       <c r="K284" t="inlineStr"/>
       <c r="L284" t="inlineStr">
         <is>
-          <t>UNII:2NDX4B6N8F</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M284" t="inlineStr">
         <is>
-          <t>HA 22</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -17761,12 +17761,12 @@
       <c r="K315" t="inlineStr"/>
       <c r="L315" t="inlineStr">
         <is>
-          <t>CHEBI:76007</t>
+          <t>CHEBI:76010</t>
         </is>
       </c>
       <c r="M315" t="inlineStr">
         <is>
-          <t>dolutegravir sodium</t>
+          <t>Dolutegravir</t>
         </is>
       </c>
     </row>
@@ -17871,12 +17871,12 @@
       <c r="K317" t="inlineStr"/>
       <c r="L317" t="inlineStr">
         <is>
-          <t>UNII:2NDX4B6N8F</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M317" t="inlineStr">
         <is>
-          <t>HA 22</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -18696,12 +18696,12 @@
       <c r="K332" t="inlineStr"/>
       <c r="L332" t="inlineStr">
         <is>
-          <t>CHEBI:71197</t>
+          <t>CHEBI:71200</t>
         </is>
       </c>
       <c r="M332" t="inlineStr">
         <is>
-          <t>tofacitinib citrate</t>
+          <t>Tofacitinib</t>
         </is>
       </c>
     </row>
@@ -18971,12 +18971,12 @@
       <c r="K337" t="inlineStr"/>
       <c r="L337" t="inlineStr">
         <is>
-          <t>CHEBI:71217</t>
+          <t>CHEBI:71219</t>
         </is>
       </c>
       <c r="M337" t="inlineStr">
         <is>
-          <t>pazopanib hydrochloride</t>
+          <t>Pazopanib</t>
         </is>
       </c>
     </row>
@@ -19411,12 +19411,12 @@
       <c r="K345" t="inlineStr"/>
       <c r="L345" t="inlineStr">
         <is>
-          <t>CHEBI:31934</t>
+          <t>CHEBI:50275</t>
         </is>
       </c>
       <c r="M345" t="inlineStr">
         <is>
-          <t>Omeprazole sodium</t>
+          <t>Esomeprazole</t>
         </is>
       </c>
     </row>
@@ -19466,12 +19466,12 @@
       <c r="K346" t="inlineStr"/>
       <c r="L346" t="inlineStr">
         <is>
-          <t>CHEBI:64311</t>
+          <t>CHEBI:64321</t>
         </is>
       </c>
       <c r="M346" t="inlineStr">
         <is>
-          <t>fosaprepitant dimeglumine</t>
+          <t>Fosaprepitant</t>
         </is>
       </c>
     </row>
@@ -20511,12 +20511,12 @@
       <c r="K365" t="inlineStr"/>
       <c r="L365" t="inlineStr">
         <is>
-          <t>CHEBI:2566</t>
+          <t>CHEBI:2567</t>
         </is>
       </c>
       <c r="M365" t="inlineStr">
         <is>
-          <t>alendronate sodium trihydrate</t>
+          <t>Alendronic acid</t>
         </is>
       </c>
     </row>
@@ -21666,12 +21666,12 @@
       <c r="K386" t="inlineStr"/>
       <c r="L386" t="inlineStr">
         <is>
-          <t>CHEBI:4462</t>
+          <t>CHEBI:41879</t>
         </is>
       </c>
       <c r="M386" t="inlineStr">
         <is>
-          <t>dexamethasone sodium phosphate</t>
+          <t>Dexamethasone</t>
         </is>
       </c>
     </row>
@@ -21996,12 +21996,12 @@
       <c r="K392" t="inlineStr"/>
       <c r="L392" t="inlineStr">
         <is>
-          <t>CHEBI:53777</t>
+          <t>PUBCHEM.COMPOUND:9939627</t>
         </is>
       </c>
       <c r="M392" t="inlineStr">
         <is>
-          <t>aliskiren fumarate</t>
+          <t>ALISKIREN FUMARATE</t>
         </is>
       </c>
     </row>
@@ -22821,12 +22821,12 @@
       <c r="K407" t="inlineStr"/>
       <c r="L407" t="inlineStr">
         <is>
-          <t>CHEBI:59936</t>
+          <t>UNII:780F0P8N4I</t>
         </is>
       </c>
       <c r="M407" t="inlineStr">
         <is>
-          <t>ciprofloxacin hydrochloride hydrate</t>
+          <t>miriplatin</t>
         </is>
       </c>
     </row>
@@ -24141,12 +24141,12 @@
       <c r="K431" t="inlineStr"/>
       <c r="L431" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M431" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -25021,12 +25021,12 @@
       <c r="K447" t="inlineStr"/>
       <c r="L447" t="inlineStr">
         <is>
-          <t>CHEBI:9180</t>
+          <t>UNII:HOY74VZE0M</t>
         </is>
       </c>
       <c r="M447" t="inlineStr">
         <is>
-          <t>Sodium salicylate</t>
+          <t>gadoxetate</t>
         </is>
       </c>
     </row>
@@ -25610,12 +25610,12 @@
       <c r="K458" t="inlineStr"/>
       <c r="L458" t="inlineStr">
         <is>
-          <t>CHEBI:7008</t>
+          <t>CHEBI:63611</t>
         </is>
       </c>
       <c r="M458" t="inlineStr">
         <is>
-          <t>moxifloxacin hydrochloride</t>
+          <t>Moxifloxacin</t>
         </is>
       </c>
     </row>
@@ -26299,12 +26299,12 @@
       <c r="K471" t="inlineStr"/>
       <c r="L471" t="inlineStr">
         <is>
-          <t>CHEBI:2676</t>
+          <t>['Error']</t>
         </is>
       </c>
       <c r="M471" t="inlineStr">
         <is>
-          <t>Amoxicillin</t>
+          <t>['Error']</t>
         </is>
       </c>
     </row>
@@ -26352,12 +26352,12 @@
       <c r="K472" t="inlineStr"/>
       <c r="L472" t="inlineStr">
         <is>
-          <t>PUBCHEM.COMPOUND:121480897</t>
+          <t>PUBCHEM.COMPOUND:6475367</t>
         </is>
       </c>
       <c r="M472" t="inlineStr">
         <is>
-          <t>Ciclosporin V (Cyclosporin Impurity E)</t>
+          <t>[MeVal]5-Ciclosporin</t>
         </is>
       </c>
     </row>
@@ -26511,12 +26511,12 @@
       <c r="K475" t="inlineStr"/>
       <c r="L475" t="inlineStr">
         <is>
-          <t>UNII:75R0U2568I</t>
+          <t>UNII:RWM8CCW8GP</t>
         </is>
       </c>
       <c r="M475" t="inlineStr">
         <is>
-          <t>Octreotide Acetate</t>
+          <t>Octreotide</t>
         </is>
       </c>
     </row>
@@ -26776,12 +26776,12 @@
       <c r="K480" t="inlineStr"/>
       <c r="L480" t="inlineStr">
         <is>
-          <t>CHEBI:7003</t>
+          <t>CHEBI:17303</t>
         </is>
       </c>
       <c r="M480" t="inlineStr">
         <is>
-          <t>morphine sulfate</t>
+          <t>Morphine</t>
         </is>
       </c>
     </row>
@@ -27147,12 +27147,12 @@
       <c r="K487" t="inlineStr"/>
       <c r="L487" t="inlineStr">
         <is>
-          <t>UNII:19364RWW06</t>
+          <t>CHEBI:5971</t>
         </is>
       </c>
       <c r="M487" t="inlineStr">
         <is>
-          <t>maropitant citrate anhydrous</t>
+          <t>irinotecan hydrochloride (anhydrous)</t>
         </is>
       </c>
     </row>
@@ -27467,12 +27467,12 @@
       <c r="K493" t="inlineStr"/>
       <c r="L493" t="inlineStr">
         <is>
-          <t>CHEBI:59936</t>
+          <t>CHEBI:36560</t>
         </is>
       </c>
       <c r="M493" t="inlineStr">
         <is>
-          <t>ciprofloxacin hydrochloride hydrate</t>
+          <t>Zinc oxide</t>
         </is>
       </c>
     </row>
@@ -28787,12 +28787,12 @@
       <c r="K517" t="inlineStr"/>
       <c r="L517" t="inlineStr">
         <is>
-          <t>CHEBI:7963</t>
+          <t>CHEBI:18208</t>
         </is>
       </c>
       <c r="M517" t="inlineStr">
         <is>
-          <t>benzylpenicillin potassium</t>
+          <t>Penicillin G</t>
         </is>
       </c>
     </row>
@@ -29172,12 +29172,12 @@
       <c r="K524" t="inlineStr"/>
       <c r="L524" t="inlineStr">
         <is>
-          <t>UNII:Y6581YAW9V</t>
+          <t>UNII:5YL4IQ1078</t>
         </is>
       </c>
       <c r="M524" t="inlineStr">
         <is>
-          <t>OSILODROSTAT PHOSPHATE</t>
+          <t>Osilodrostat</t>
         </is>
       </c>
     </row>
@@ -29392,12 +29392,12 @@
       <c r="K528" t="inlineStr"/>
       <c r="L528" t="inlineStr">
         <is>
-          <t>PUBCHEM.COMPOUND:162461035</t>
+          <t>CHEBI:231693</t>
         </is>
       </c>
       <c r="M528" t="inlineStr">
         <is>
-          <t>Capmatinib hydrochloride hydrate</t>
+          <t>Capmatinib</t>
         </is>
       </c>
     </row>
@@ -29612,12 +29612,12 @@
       <c r="K532" t="inlineStr"/>
       <c r="L532" t="inlineStr">
         <is>
-          <t>CHEBI:76015</t>
+          <t>CHEBI:76016</t>
         </is>
       </c>
       <c r="M532" t="inlineStr">
         <is>
-          <t>vortioxetine hydrobromide</t>
+          <t>Vortioxetine</t>
         </is>
       </c>
     </row>
@@ -30437,12 +30437,12 @@
       <c r="K547" t="inlineStr"/>
       <c r="L547" t="inlineStr">
         <is>
-          <t>UNII:P188ANX8CK</t>
+          <t>UNII:5384HK7574</t>
         </is>
       </c>
       <c r="M547" t="inlineStr">
         <is>
-          <t>Trastuzumab</t>
+          <t>Trastuzumab deruxtecan</t>
         </is>
       </c>
     </row>
@@ -30492,12 +30492,12 @@
       <c r="K548" t="inlineStr"/>
       <c r="L548" t="inlineStr">
         <is>
-          <t>UNII:P188ANX8CK</t>
+          <t>UNII:5384HK7574</t>
         </is>
       </c>
       <c r="M548" t="inlineStr">
         <is>
-          <t>Trastuzumab</t>
+          <t>Trastuzumab deruxtecan</t>
         </is>
       </c>
     </row>
@@ -32527,12 +32527,12 @@
       <c r="K585" t="inlineStr"/>
       <c r="L585" t="inlineStr">
         <is>
-          <t>CHEBI:75991</t>
+          <t>CHEBI:75998</t>
         </is>
       </c>
       <c r="M585" t="inlineStr">
         <is>
-          <t>trametinib dimethyl sulfoxide</t>
+          <t>Trametinib</t>
         </is>
       </c>
     </row>
@@ -32912,12 +32912,12 @@
       <c r="K592" t="inlineStr"/>
       <c r="L592" t="inlineStr">
         <is>
-          <t>CHEBI:65344</t>
+          <t>CHEBI:65346</t>
         </is>
       </c>
       <c r="M592" t="inlineStr">
         <is>
-          <t>aclidinium bromide</t>
+          <t>Aclidinium</t>
         </is>
       </c>
     </row>
@@ -33187,12 +33187,12 @@
       <c r="K597" t="inlineStr"/>
       <c r="L597" t="inlineStr">
         <is>
-          <t>CHEBI:62268</t>
+          <t>CHEBI:90936</t>
         </is>
       </c>
       <c r="M597" t="inlineStr">
         <is>
-          <t>alectinib hydrochloride</t>
+          <t>Alectinib</t>
         </is>
       </c>
     </row>
@@ -33627,12 +33627,12 @@
       <c r="K605" t="inlineStr"/>
       <c r="L605" t="inlineStr">
         <is>
-          <t>PUBCHEM.COMPOUND:24936221</t>
+          <t>CHEBI:85078</t>
         </is>
       </c>
       <c r="M605" t="inlineStr">
         <is>
-          <t>Dapagliflozin propylene glycolate hydrate</t>
+          <t>Dapagliflozin</t>
         </is>
       </c>
     </row>
@@ -33792,12 +33792,12 @@
       <c r="K608" t="inlineStr"/>
       <c r="L608" t="inlineStr">
         <is>
-          <t>UNII:P188ANX8CK</t>
+          <t>UNII:5384HK7574</t>
         </is>
       </c>
       <c r="M608" t="inlineStr">
         <is>
-          <t>Trastuzumab</t>
+          <t>Trastuzumab deruxtecan</t>
         </is>
       </c>
     </row>
@@ -33847,12 +33847,12 @@
       <c r="K609" t="inlineStr"/>
       <c r="L609" t="inlineStr">
         <is>
-          <t>DRUGBANK:DB19320</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M609" t="inlineStr">
         <is>
-          <t>Influenza A virus A/Thailand/8/2022 IVR-237 (H3N2) antigen (propiolactone inactivated)</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -33902,12 +33902,12 @@
       <c r="K610" t="inlineStr"/>
       <c r="L610" t="inlineStr">
         <is>
-          <t>DRUGBANK:DB19320</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M610" t="inlineStr">
         <is>
-          <t>Influenza A virus A/Thailand/8/2022 IVR-237 (H3N2) antigen (propiolactone inactivated)</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -33957,12 +33957,12 @@
       <c r="K611" t="inlineStr"/>
       <c r="L611" t="inlineStr">
         <is>
-          <t>DRUGBANK:DB09877</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M611" t="inlineStr">
         <is>
-          <t>Corynebacterium diphtheriae</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -34177,12 +34177,12 @@
       <c r="K615" t="inlineStr"/>
       <c r="L615" t="inlineStr">
         <is>
-          <t>CHEBI:50140</t>
+          <t>CHEBI:167309</t>
         </is>
       </c>
       <c r="M615" t="inlineStr">
         <is>
-          <t>methadone hydrochloride</t>
+          <t>Methadone</t>
         </is>
       </c>
     </row>
@@ -34727,12 +34727,12 @@
       <c r="K625" t="inlineStr"/>
       <c r="L625" t="inlineStr">
         <is>
-          <t>CHEBI:71271</t>
+          <t>CHEBI:71272</t>
         </is>
       </c>
       <c r="M625" t="inlineStr">
         <is>
-          <t>saxagliptin</t>
+          <t>Saxagliptin</t>
         </is>
       </c>
     </row>
@@ -35167,12 +35167,12 @@
       <c r="K633" t="inlineStr"/>
       <c r="L633" t="inlineStr">
         <is>
-          <t>CHEBI:63112</t>
+          <t>CHEBI:63115</t>
         </is>
       </c>
       <c r="M633" t="inlineStr">
         <is>
-          <t>fingolimod hydrochloride</t>
+          <t>Fingolimod</t>
         </is>
       </c>
     </row>
@@ -35222,12 +35222,12 @@
       <c r="K634" t="inlineStr"/>
       <c r="L634" t="inlineStr">
         <is>
-          <t>CHEBI:59900</t>
+          <t>UNII:VUW370O5QE</t>
         </is>
       </c>
       <c r="M634" t="inlineStr">
         <is>
-          <t>caspofungin acetate</t>
+          <t>CASPOFUNGIN ACETATE</t>
         </is>
       </c>
     </row>
@@ -35497,12 +35497,12 @@
       <c r="K639" t="inlineStr"/>
       <c r="L639" t="inlineStr">
         <is>
-          <t>CHEBI:70743</t>
+          <t>CHEBI:70746</t>
         </is>
       </c>
       <c r="M639" t="inlineStr">
         <is>
-          <t>Rendix</t>
+          <t>Dabigatran etexilate</t>
         </is>
       </c>
     </row>
@@ -35772,12 +35772,12 @@
       <c r="K644" t="inlineStr"/>
       <c r="L644" t="inlineStr">
         <is>
-          <t>UNII:6A901E312A</t>
+          <t>['Error']</t>
         </is>
       </c>
       <c r="M644" t="inlineStr">
         <is>
-          <t>Panitumumab</t>
+          <t>['Error']</t>
         </is>
       </c>
     </row>
@@ -35937,12 +35937,12 @@
       <c r="K647" t="inlineStr"/>
       <c r="L647" t="inlineStr">
         <is>
-          <t>CHEBI:31526</t>
+          <t>CHEBI:36795</t>
         </is>
       </c>
       <c r="M647" t="inlineStr">
         <is>
-          <t>(S)-duloxetine hydrochloride</t>
+          <t>Duloxetine</t>
         </is>
       </c>
     </row>
@@ -35992,12 +35992,12 @@
       <c r="K648" t="inlineStr"/>
       <c r="L648" t="inlineStr">
         <is>
-          <t>CHEBI:90952</t>
+          <t>CHEBI:90953</t>
         </is>
       </c>
       <c r="M648" t="inlineStr">
         <is>
-          <t>sugammadex sodium</t>
+          <t>Sugammadex</t>
         </is>
       </c>
     </row>
@@ -36052,7 +36052,7 @@
       </c>
       <c r="M649" t="inlineStr">
         <is>
-          <t>Rapivab</t>
+          <t>peramivir hydrate</t>
         </is>
       </c>
     </row>
@@ -36817,12 +36817,12 @@
       <c r="K663" t="inlineStr"/>
       <c r="L663" t="inlineStr">
         <is>
-          <t>CHEBI:6993</t>
+          <t>CHEBI:50730</t>
         </is>
       </c>
       <c r="M663" t="inlineStr">
         <is>
-          <t>montelukast sodium</t>
+          <t>Montelukast</t>
         </is>
       </c>
     </row>
@@ -37514,12 +37514,12 @@
       <c r="K676" t="inlineStr"/>
       <c r="L676" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>['Error']</t>
         </is>
       </c>
       <c r="M676" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>['Error']</t>
         </is>
       </c>
     </row>
@@ -37620,12 +37620,12 @@
       <c r="K678" t="inlineStr"/>
       <c r="L678" t="inlineStr">
         <is>
-          <t>CHEBI:16027</t>
+          <t>CHEBI:16335</t>
         </is>
       </c>
       <c r="M678" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>Adenosine</t>
         </is>
       </c>
     </row>
@@ -37889,12 +37889,12 @@
       <c r="K683" t="inlineStr"/>
       <c r="L683" t="inlineStr">
         <is>
-          <t>UNII:NA1U919MRO</t>
+          <t>UNII:0P70AR5BYB</t>
         </is>
       </c>
       <c r="M683" t="inlineStr">
         <is>
-          <t>Difelikefalin</t>
+          <t>DIFELIKEFALIN ACETATE</t>
         </is>
       </c>
     </row>
@@ -38274,12 +38274,12 @@
       <c r="K690" t="inlineStr"/>
       <c r="L690" t="inlineStr">
         <is>
-          <t>DRUGBANK:DB19320</t>
+          <t>DRUGBANK:DB18750</t>
         </is>
       </c>
       <c r="M690" t="inlineStr">
         <is>
-          <t>Influenza A virus A/Thailand/8/2022 IVR-237 (H3N2) antigen (propiolactone inactivated)</t>
+          <t>Influenza A Virus A/California/122/2022 SAN-022 (H3N2) antigen (formaldehyde inactivated)</t>
         </is>
       </c>
     </row>
@@ -39374,12 +39374,12 @@
       <c r="K710" t="inlineStr"/>
       <c r="L710" t="inlineStr">
         <is>
-          <t>CHEBI:90939</t>
+          <t>CHEBI:90942</t>
         </is>
       </c>
       <c r="M710" t="inlineStr">
         <is>
-          <t>ixazomib citrate</t>
+          <t>Ixazomib</t>
         </is>
       </c>
     </row>
@@ -39594,12 +39594,12 @@
       <c r="K714" t="inlineStr"/>
       <c r="L714" t="inlineStr">
         <is>
-          <t>CHEBI:31602</t>
+          <t>CHEBI:119915</t>
         </is>
       </c>
       <c r="M714" t="inlineStr">
         <is>
-          <t>fentanyl citrate</t>
+          <t>Fentanyl</t>
         </is>
       </c>
     </row>
@@ -40419,12 +40419,12 @@
       <c r="K729" t="inlineStr"/>
       <c r="L729" t="inlineStr">
         <is>
-          <t>CHEBI:53509</t>
+          <t>CHEBI:114785</t>
         </is>
       </c>
       <c r="M729" t="inlineStr">
         <is>
-          <t>Tarceva</t>
+          <t>Erlotinib</t>
         </is>
       </c>
     </row>
@@ -40578,12 +40578,12 @@
       <c r="K732" t="inlineStr"/>
       <c r="L732" t="inlineStr">
         <is>
-          <t>PUBCHEM.COMPOUND:6440720</t>
+          <t>PUBCHEM.COMPOUND:170190</t>
         </is>
       </c>
       <c r="M732" t="inlineStr">
         <is>
-          <t>avobenzone, ensulizole, enzacamene drug combination</t>
+          <t>aluminum hydroxide, magnesium hydroxide, simethicone drug combination</t>
         </is>
       </c>
     </row>
@@ -41110,12 +41110,12 @@
       <c r="K742" t="inlineStr"/>
       <c r="L742" t="inlineStr">
         <is>
-          <t>UNII:WYD79216A6</t>
+          <t>UNII:50605O2ZNS</t>
         </is>
       </c>
       <c r="M742" t="inlineStr">
         <is>
-          <t>Tenapanor</t>
+          <t>TENAPANOR HYDROCHLORIDE</t>
         </is>
       </c>
     </row>
@@ -41385,12 +41385,12 @@
       <c r="K747" t="inlineStr"/>
       <c r="L747" t="inlineStr">
         <is>
-          <t>CHEBI:70732</t>
+          <t>CHEBI:70735</t>
         </is>
       </c>
       <c r="M747" t="inlineStr">
         <is>
-          <t>lurasidone hydrochloride</t>
+          <t>Lurasidone</t>
         </is>
       </c>
     </row>
@@ -41605,12 +41605,12 @@
       <c r="K751" t="inlineStr"/>
       <c r="L751" t="inlineStr">
         <is>
-          <t>UNII:P188ANX8CK</t>
+          <t>UNII:5384HK7574</t>
         </is>
       </c>
       <c r="M751" t="inlineStr">
         <is>
-          <t>Trastuzumab</t>
+          <t>Trastuzumab deruxtecan</t>
         </is>
       </c>
     </row>
@@ -42536,12 +42536,12 @@
       <c r="K768" t="inlineStr"/>
       <c r="L768" t="inlineStr">
         <is>
-          <t>CHEBI:31387</t>
+          <t>CHEBI:59224</t>
         </is>
       </c>
       <c r="M768" t="inlineStr">
         <is>
-          <t>Cetrotide</t>
+          <t>Cetrorelix</t>
         </is>
       </c>
     </row>
@@ -42864,12 +42864,12 @@
       <c r="K774" t="inlineStr"/>
       <c r="L774" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M774" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -43139,12 +43139,12 @@
       <c r="K779" t="inlineStr"/>
       <c r="L779" t="inlineStr">
         <is>
-          <t>CHEBI:31602</t>
+          <t>CHEBI:119915</t>
         </is>
       </c>
       <c r="M779" t="inlineStr">
         <is>
-          <t>fentanyl citrate</t>
+          <t>Fentanyl</t>
         </is>
       </c>
     </row>
@@ -43249,12 +43249,12 @@
       <c r="K781" t="inlineStr"/>
       <c r="L781" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M781" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -43799,12 +43799,12 @@
       <c r="K791" t="inlineStr"/>
       <c r="L791" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M791" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -43854,12 +43854,12 @@
       <c r="K792" t="inlineStr"/>
       <c r="L792" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M792" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -43909,12 +43909,12 @@
       <c r="K793" t="inlineStr"/>
       <c r="L793" t="inlineStr">
         <is>
-          <t>UNII:6892UQT2GK</t>
+          <t>UNII:U50VWW6XH6</t>
         </is>
       </c>
       <c r="M793" t="inlineStr">
         <is>
-          <t>Susoctocog alfa</t>
+          <t>Simoctocog alfa</t>
         </is>
       </c>
     </row>
@@ -44675,12 +44675,12 @@
       <c r="K807" t="inlineStr"/>
       <c r="L807" t="inlineStr">
         <is>
-          <t>CHEBI:80105</t>
+          <t>CHEBI:600520</t>
         </is>
       </c>
       <c r="M807" t="inlineStr">
         <is>
-          <t>micafungin sodium</t>
+          <t>Micafungin</t>
         </is>
       </c>
     </row>
@@ -44838,12 +44838,12 @@
       <c r="K810" t="inlineStr"/>
       <c r="L810" t="inlineStr">
         <is>
-          <t>CHEBI:85977</t>
+          <t>CHEBI:85978</t>
         </is>
       </c>
       <c r="M810" t="inlineStr">
         <is>
-          <t>isavuconazonium sulfate</t>
+          <t>Isavuconazonium</t>
         </is>
       </c>
     </row>
@@ -46321,12 +46321,12 @@
       <c r="K837" t="inlineStr"/>
       <c r="L837" t="inlineStr">
         <is>
-          <t>CHEBI:4026</t>
+          <t>CHEBI:4027</t>
         </is>
       </c>
       <c r="M837" t="inlineStr">
         <is>
-          <t>cyclophosphamide hydrate</t>
+          <t>Cyclophosphamide</t>
         </is>
       </c>
     </row>
@@ -46706,7 +46706,7 @@
       <c r="K844" t="inlineStr"/>
       <c r="L844" t="inlineStr">
         <is>
-          <t>PUBCHEM.COMPOUND:135436482</t>
+          <t>PUBCHEM.COMPOUND:135430945</t>
         </is>
       </c>
       <c r="M844" t="inlineStr">
@@ -46981,12 +46981,12 @@
       <c r="K849" t="inlineStr"/>
       <c r="L849" t="inlineStr">
         <is>
-          <t>CHEBI:31456</t>
+          <t>CHEBI:41977</t>
         </is>
       </c>
       <c r="M849" t="inlineStr">
         <is>
-          <t>Daunorubicin hydrochloride</t>
+          <t>Daunorubicin</t>
         </is>
       </c>
     </row>
@@ -47476,12 +47476,12 @@
       <c r="K858" t="inlineStr"/>
       <c r="L858" t="inlineStr">
         <is>
-          <t>CHEBI:2417</t>
+          <t>CHEBI:15355</t>
         </is>
       </c>
       <c r="M858" t="inlineStr">
         <is>
-          <t>acetylcholine chloride</t>
+          <t>Acetylcholine</t>
         </is>
       </c>
     </row>
@@ -47531,12 +47531,12 @@
       <c r="K859" t="inlineStr"/>
       <c r="L859" t="inlineStr">
         <is>
-          <t>UNII:2NDX4B6N8F</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M859" t="inlineStr">
         <is>
-          <t>HA 22</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -47586,12 +47586,12 @@
       <c r="K860" t="inlineStr"/>
       <c r="L860" t="inlineStr">
         <is>
-          <t>UNII:2NDX4B6N8F</t>
+          <t>DRUGBANK:DB15507</t>
         </is>
       </c>
       <c r="M860" t="inlineStr">
         <is>
-          <t>HA 22</t>
+          <t>Influenza B virus B/Singapore/INFTT-16-0610/2016 antigen (MDCK cell derived, propiolactone inactivated)</t>
         </is>
       </c>
     </row>
@@ -47916,12 +47916,12 @@
       <c r="K866" t="inlineStr"/>
       <c r="L866" t="inlineStr">
         <is>
-          <t>CHEBI:59936</t>
+          <t>CHEBI:100241</t>
         </is>
       </c>
       <c r="M866" t="inlineStr">
         <is>
-          <t>ciprofloxacin hydrochloride hydrate</t>
+          <t>Ciprofloxacin</t>
         </is>
       </c>
     </row>
@@ -49511,12 +49511,12 @@
       <c r="K895" t="inlineStr"/>
       <c r="L895" t="inlineStr">
         <is>
-          <t>CHEBI:31690</t>
+          <t>CHEBI:45783</t>
         </is>
       </c>
       <c r="M895" t="inlineStr">
         <is>
-          <t>imatinib methanesulfonate</t>
+          <t>Imatinib</t>
         </is>
       </c>
     </row>
@@ -49731,12 +49731,12 @@
       <c r="K899" t="inlineStr"/>
       <c r="L899" t="inlineStr">
         <is>
-          <t>CHEBI:9984</t>
+          <t>CHEBI:27375</t>
         </is>
       </c>
       <c r="M899" t="inlineStr">
         <is>
-          <t>vincaleukoblastine sulfate</t>
+          <t>Vinblastine</t>
         </is>
       </c>
     </row>
@@ -50226,7 +50226,7 @@
       <c r="K908" t="inlineStr"/>
       <c r="L908" t="inlineStr">
         <is>
-          <t>CHEBI:31695</t>
+          <t>CHEBI:90117</t>
         </is>
       </c>
       <c r="M908" t="inlineStr">
@@ -50336,12 +50336,12 @@
       <c r="K910" t="inlineStr"/>
       <c r="L910" t="inlineStr">
         <is>
-          <t>CHEBI:9423</t>
+          <t>CHEBI:33353</t>
         </is>
       </c>
       <c r="M910" t="inlineStr">
         <is>
-          <t>Cardiolite (TN)</t>
+          <t>technetium atom</t>
         </is>
       </c>
     </row>
@@ -50391,12 +50391,12 @@
       <c r="K911" t="inlineStr"/>
       <c r="L911" t="inlineStr">
         <is>
-          <t>CHEBI:9423</t>
+          <t>CHEBI:33353</t>
         </is>
       </c>
       <c r="M911" t="inlineStr">
         <is>
-          <t>Cardiolite (TN)</t>
+          <t>technetium atom</t>
         </is>
       </c>
     </row>
@@ -50446,12 +50446,12 @@
       <c r="K912" t="inlineStr"/>
       <c r="L912" t="inlineStr">
         <is>
-          <t>CHEBI:9423</t>
+          <t>CHEBI:33353</t>
         </is>
       </c>
       <c r="M912" t="inlineStr">
         <is>
-          <t>Cardiolite (TN)</t>
+          <t>technetium atom</t>
         </is>
       </c>
     </row>
@@ -50721,12 +50721,12 @@
       <c r="K917" t="inlineStr"/>
       <c r="L917" t="inlineStr">
         <is>
-          <t>CHEBI:32120</t>
+          <t>CHEBI:59560</t>
         </is>
       </c>
       <c r="M917" t="inlineStr">
         <is>
-          <t>sapropterin dihydrochloride</t>
+          <t>Sapropterin</t>
         </is>
       </c>
     </row>
@@ -51271,12 +51271,12 @@
       <c r="K927" t="inlineStr"/>
       <c r="L927" t="inlineStr">
         <is>
-          <t>UNII:P188ANX8CK</t>
+          <t>UNII:5384HK7574</t>
         </is>
       </c>
       <c r="M927" t="inlineStr">
         <is>
-          <t>Trastuzumab</t>
+          <t>Trastuzumab deruxtecan</t>
         </is>
       </c>
     </row>
@@ -52261,12 +52261,12 @@
       <c r="K945" t="inlineStr"/>
       <c r="L945" t="inlineStr">
         <is>
-          <t>CHEBI:3755</t>
+          <t>CHEBI:47780</t>
         </is>
       </c>
       <c r="M945" t="inlineStr">
         <is>
-          <t>clomipramine hydrochloride</t>
+          <t>Clomipramine</t>
         </is>
       </c>
     </row>
@@ -52756,12 +52756,12 @@
       <c r="K954" t="inlineStr"/>
       <c r="L954" t="inlineStr">
         <is>
-          <t>CHEBI:7963</t>
+          <t>CHEBI:18208</t>
         </is>
       </c>
       <c r="M954" t="inlineStr">
         <is>
-          <t>benzylpenicillin potassium</t>
+          <t>Penicillin G</t>
         </is>
       </c>
     </row>
@@ -52811,12 +52811,12 @@
       <c r="K955" t="inlineStr"/>
       <c r="L955" t="inlineStr">
         <is>
-          <t>CHEBI:53509</t>
+          <t>CHEBI:114785</t>
         </is>
       </c>
       <c r="M955" t="inlineStr">
         <is>
-          <t>Tarceva</t>
+          <t>Erlotinib</t>
         </is>
       </c>
     </row>
@@ -52921,12 +52921,12 @@
       <c r="K957" t="inlineStr"/>
       <c r="L957" t="inlineStr">
         <is>
-          <t>CHEBI:94758</t>
+          <t>CHEBI:32107</t>
         </is>
       </c>
       <c r="M957" t="inlineStr">
         <is>
-          <t>Roxane</t>
+          <t>TZU 0460</t>
         </is>
       </c>
     </row>
@@ -52976,12 +52976,12 @@
       <c r="K958" t="inlineStr"/>
       <c r="L958" t="inlineStr">
         <is>
-          <t>CHEBI:5091</t>
+          <t>CHEBI:75984</t>
         </is>
       </c>
       <c r="M958" t="inlineStr">
         <is>
-          <t>flecainide acetate</t>
+          <t>Flecainide</t>
         </is>
       </c>
     </row>
@@ -53746,12 +53746,12 @@
       <c r="K972" t="inlineStr"/>
       <c r="L972" t="inlineStr">
         <is>
-          <t>CHEBI:31934</t>
+          <t>CHEBI:50275</t>
         </is>
       </c>
       <c r="M972" t="inlineStr">
         <is>
-          <t>Omeprazole sodium</t>
+          <t>Esomeprazole</t>
         </is>
       </c>
     </row>
@@ -54186,12 +54186,12 @@
       <c r="K980" t="inlineStr"/>
       <c r="L980" t="inlineStr">
         <is>
-          <t>CHEBI:5781</t>
+          <t>CHEBI:17650</t>
         </is>
       </c>
       <c r="M980" t="inlineStr">
         <is>
-          <t>cortisol sodium phosphate</t>
+          <t>Hydrocortisone</t>
         </is>
       </c>
     </row>
@@ -54461,12 +54461,12 @@
       <c r="K985" t="inlineStr"/>
       <c r="L985" t="inlineStr">
         <is>
-          <t>CHEBI:6770</t>
+          <t>CHEBI:43968</t>
         </is>
       </c>
       <c r="M985" t="inlineStr">
         <is>
-          <t>MEROPENEM</t>
+          <t>Meropenem</t>
         </is>
       </c>
     </row>
@@ -54681,12 +54681,12 @@
       <c r="K989" t="inlineStr"/>
       <c r="L989" t="inlineStr">
         <is>
-          <t>CHEBI:4667</t>
+          <t>CHEBI:39867</t>
         </is>
       </c>
       <c r="M989" t="inlineStr">
         <is>
-          <t>valproate semisodium</t>
+          <t>Valproic acid</t>
         </is>
       </c>
     </row>
@@ -54791,12 +54791,12 @@
       <c r="K991" t="inlineStr"/>
       <c r="L991" t="inlineStr">
         <is>
-          <t>CHEBI:4026</t>
+          <t>CHEBI:4027</t>
         </is>
       </c>
       <c r="M991" t="inlineStr">
         <is>
-          <t>cyclophosphamide hydrate</t>
+          <t>Cyclophosphamide</t>
         </is>
       </c>
     </row>
@@ -55066,12 +55066,12 @@
       <c r="K996" t="inlineStr"/>
       <c r="L996" t="inlineStr">
         <is>
-          <t>CHEBI:3514</t>
+          <t>CHEBI:29007</t>
         </is>
       </c>
       <c r="M996" t="inlineStr">
         <is>
-          <t>Ceftriaxone disodium salt hemiheptahydrate</t>
+          <t>Ceftriaxone</t>
         </is>
       </c>
     </row>
@@ -55891,12 +55891,12 @@
       <c r="K1011" t="inlineStr"/>
       <c r="L1011" t="inlineStr">
         <is>
-          <t>CHEBI:3498</t>
+          <t>CHEBI:204928</t>
         </is>
       </c>
       <c r="M1011" t="inlineStr">
         <is>
-          <t>cefotaxime sodium</t>
+          <t>Cefotaxime</t>
         </is>
       </c>
     </row>
@@ -56881,12 +56881,12 @@
       <c r="K1029" t="inlineStr"/>
       <c r="L1029" t="inlineStr">
         <is>
-          <t>CHEBI:31934</t>
+          <t>CHEBI:6909</t>
         </is>
       </c>
       <c r="M1029" t="inlineStr">
         <is>
-          <t>Omeprazole sodium</t>
+          <t>Metronidazole</t>
         </is>
       </c>
     </row>
@@ -56936,12 +56936,12 @@
       <c r="K1030" t="inlineStr"/>
       <c r="L1030" t="inlineStr">
         <is>
-          <t>CHEBI:31281</t>
+          <t>CHEBI:71204</t>
         </is>
       </c>
       <c r="M1030" t="inlineStr">
         <is>
-          <t>bepotastine besylate</t>
+          <t>bepotastine</t>
         </is>
       </c>
     </row>
@@ -58114,12 +58114,12 @@
       <c r="K1052" t="inlineStr"/>
       <c r="L1052" t="inlineStr">
         <is>
-          <t>CHEBI:32296</t>
+          <t>CHEBI:480999</t>
         </is>
       </c>
       <c r="M1052" t="inlineStr">
         <is>
-          <t>vinorelbine L-tartrate</t>
+          <t>Vinorelbine</t>
         </is>
       </c>
     </row>
@@ -58220,12 +58220,12 @@
       <c r="K1054" t="inlineStr"/>
       <c r="L1054" t="inlineStr">
         <is>
-          <t>CHEBI:4462</t>
+          <t>PUBCHEM.COMPOUND:23667621</t>
         </is>
       </c>
       <c r="M1054" t="inlineStr">
         <is>
-          <t>dexamethasone sodium phosphate</t>
+          <t>DEXAMETHASONE SODIUM PHOSPHATE</t>
         </is>
       </c>
     </row>
@@ -58326,12 +58326,12 @@
       <c r="K1056" t="inlineStr"/>
       <c r="L1056" t="inlineStr">
         <is>
-          <t>CHEBI:59936</t>
+          <t>CHEBI:100241</t>
         </is>
       </c>
       <c r="M1056" t="inlineStr">
         <is>
-          <t>ciprofloxacin hydrochloride hydrate</t>
+          <t>Ciprofloxacin</t>
         </is>
       </c>
     </row>
@@ -58379,12 +58379,12 @@
       <c r="K1057" t="inlineStr"/>
       <c r="L1057" t="inlineStr">
         <is>
-          <t>UNII:1RXS4UE564</t>
+          <t>['Error']</t>
         </is>
       </c>
       <c r="M1057" t="inlineStr">
         <is>
-          <t>Alteplase</t>
+          <t>['Error']</t>
         </is>
       </c>
     </row>
@@ -58485,12 +58485,12 @@
       <c r="K1059" t="inlineStr"/>
       <c r="L1059" t="inlineStr">
         <is>
-          <t>CHEBI:31934</t>
+          <t>CHEBI:2676</t>
         </is>
       </c>
       <c r="M1059" t="inlineStr">
         <is>
-          <t>Omeprazole sodium</t>
+          <t>Amoxicillin</t>
         </is>
       </c>
     </row>
@@ -58697,12 +58697,12 @@
       <c r="K1063" t="inlineStr"/>
       <c r="L1063" t="inlineStr">
         <is>
-          <t>CHEBI:6770</t>
+          <t>CHEBI:43968</t>
         </is>
       </c>
       <c r="M1063" t="inlineStr">
         <is>
-          <t>MEROPENEM</t>
+          <t>Meropenem</t>
         </is>
       </c>
     </row>
@@ -58750,12 +58750,12 @@
       <c r="K1064" t="inlineStr"/>
       <c r="L1064" t="inlineStr">
         <is>
-          <t>CHEBI:31368</t>
+          <t>CHEBI:478164</t>
         </is>
       </c>
       <c r="M1064" t="inlineStr">
         <is>
-          <t>cefepime hydrochloride</t>
+          <t>Cefepime</t>
         </is>
       </c>
     </row>
@@ -58803,12 +58803,12 @@
       <c r="K1065" t="inlineStr"/>
       <c r="L1065" t="inlineStr">
         <is>
-          <t>PUBCHEM.COMPOUND:20832750</t>
+          <t>PUBCHEM.COMPOUND:131750191</t>
         </is>
       </c>
       <c r="M1065" t="inlineStr">
         <is>
-          <t>Bleomycin hydrochloride</t>
+          <t>Bleomycin Hydrochloride</t>
         </is>
       </c>
     </row>
@@ -59068,12 +59068,12 @@
       <c r="K1070" t="inlineStr"/>
       <c r="L1070" t="inlineStr">
         <is>
-          <t>CHEBI:2361</t>
+          <t>CHEBI:421707</t>
         </is>
       </c>
       <c r="M1070" t="inlineStr">
         <is>
-          <t>abacavir sulfate</t>
+          <t>Abacavir</t>
         </is>
       </c>
     </row>

</xml_diff>